<commit_message>
DevBoard update 8/2/2019 11:59PM
</commit_message>
<xml_diff>
--- a/Karman Eagle/Karman Projects/Dev Board/Current/Rev 1/Bill of Materials/1906152158-Dev Board BOM.xlsx
+++ b/Karman Eagle/Karman Projects/Dev Board/Current/Rev 1/Bill of Materials/1906152158-Dev Board BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\Videos\David's Laptop GrabCAD\EAGLE\karman-pcb\Karman Eagle\Karman Projects\Dev Board\Current\Rev 1\Bill of Materials\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C658ADD0-809A-4A4D-A39E-B47EFF3D7630}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22530287-9428-461D-AD69-69E3FD04962D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7620" xr2:uid="{C93AA0FA-E9BB-40AA-9745-29DE001A94DD}"/>
   </bookViews>
@@ -974,8 +974,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{638B8DB4-69DD-440E-99F6-9B35280CD1CD}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>